<commit_message>
added postcards from 2011
</commit_message>
<xml_diff>
--- a/vending/Vending Pay-Off.xlsx
+++ b/vending/Vending Pay-Off.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr date1904="1"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="10200"/>
+    <workbookView xWindow="8580" yWindow="-29960" windowWidth="40380" windowHeight="28880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Table 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -37,12 +42,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mmm\ d\,\ yyyy\ h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="mmm\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -57,6 +62,18 @@
       <b/>
       <sz val="10"/>
       <color indexed="9"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -125,8 +142,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
@@ -172,7 +237,23 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -252,6 +333,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -277,6 +367,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -284,20 +375,22 @@
         </a:ln>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11934279720411292"/>
-          <c:y val="6.0394171158712727E-2"/>
-          <c:w val="0.84439082211497785"/>
-          <c:h val="0.83658322279607522"/>
+          <c:x val="0.119342797204113"/>
+          <c:y val="0.0603941711587127"/>
+          <c:w val="0.844390822114978"/>
+          <c:h val="0.836583222796075"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -322,13 +415,14 @@
           <c:trendline>
             <c:name>Debt Projection</c:name>
             <c:trendlineType val="linear"/>
-            <c:forward val="1"/>
+            <c:forward val="1.0"/>
+            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.8965749116071232E-2"/>
-                  <c:y val="3.0589120672712133E-2"/>
+                  <c:x val="-0.0489657491160712"/>
+                  <c:y val="0.0305891206727121"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -336,76 +430,85 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$C$7:$C$25</c:f>
+              <c:f>'Sheet 1 - Table 1'!$C$7:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61</c:v>
+                  <c:v>61.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>91</c:v>
+                  <c:v>91.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>122</c:v>
+                  <c:v>122.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>153</c:v>
+                  <c:v>153.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>181</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>212</c:v>
+                  <c:v>212.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>242</c:v>
+                  <c:v>242.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>273</c:v>
+                  <c:v>273.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>303</c:v>
+                  <c:v>303.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>334</c:v>
+                  <c:v>334.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>365</c:v>
+                  <c:v>365.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>395</c:v>
+                  <c:v>395.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>426</c:v>
+                  <c:v>426.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>456</c:v>
+                  <c:v>456.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>487</c:v>
+                  <c:v>487.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>518</c:v>
+                  <c:v>518.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>539</c:v>
+                  <c:v>546.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>577.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>607.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>624.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$D$7:$D$25</c:f>
+              <c:f>'Sheet 1 - Table 1'!$D$7:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>6487.82</c:v>
                 </c:pt>
@@ -461,23 +564,43 @@
                   <c:v>5458.44</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5472.57</c:v>
+                  <c:v>5399.57</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5328.18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5395.66</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5277.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="72554752"/>
-        <c:axId val="72564736"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="769343592"/>
+        <c:axId val="769346952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72554752"/>
+        <c:axId val="769343592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
         <c:spPr>
           <a:ln w="12700">
@@ -504,16 +627,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72564736"/>
+        <c:crossAx val="769346952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72564736"/>
+        <c:axId val="769346952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0"/>
+          <c:min val="0.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -527,6 +651,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="9525">
@@ -550,10 +675,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72554752"/>
+        <c:crossAx val="769343592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1300"/>
+        <c:majorUnit val="1300.0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -564,6 +689,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -590,7 +716,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000022" r="0.75000000000000022" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -600,7 +726,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="4"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="104"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="4"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -619,11 +753,14 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -640,45 +777,65 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$O$4:$O$5</c:f>
+              <c:f>'Sheet 1 - Table 1'!$O$4:$O$9</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>39098</c:v>
+                  <c:v>39098.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39133</c:v>
+                  <c:v>39133.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39191.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39218.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$P$4:$P$5</c:f>
+              <c:f>'Sheet 1 - Table 1'!$P$4:$P$9</c:f>
               <c:numCache>
                 <c:formatCode>mmm\ d\,\ yyyy\ h:mm:ss\ AM/PM</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>42078.989200863929</c:v>
+                  <c:v>42078.98920086393</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42063.260533104039</c:v>
+                  <c:v>42063.26053310404</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41938.89890894048</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42035.53698571733</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="90536576"/>
-        <c:axId val="90535040"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="795896056"/>
+        <c:axId val="795902136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90536576"/>
+        <c:axId val="795896056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:minorGridlines>
@@ -711,8 +868,10 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
@@ -727,15 +886,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90535040"/>
+        <c:crossAx val="795902136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90535040"/>
+        <c:axId val="795902136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:minorGridlines>
@@ -768,8 +928,10 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
@@ -784,12 +946,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90536576"/>
+        <c:crossAx val="795896056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -811,7 +975,7 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>654845</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>130968</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -837,13 +1001,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>83343</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>142872</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>226218</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>214313</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1213,34 +1377,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="20.100000000000001" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.125" style="1" customWidth="1"/>
-    <col min="4" max="14" width="10.25" style="1"/>
-    <col min="15" max="15" width="13.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="10.25" style="1"/>
-    <col min="19" max="19" width="20.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="10.25" style="1"/>
+    <col min="1" max="1" width="10.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="1" customWidth="1"/>
+    <col min="4" max="14" width="10.140625" style="1"/>
+    <col min="15" max="15" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.140625" style="1"/>
+    <col min="19" max="19" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="12.75">
+    <row r="1" spans="1:16" ht="13">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:16" ht="12.75">
+    <row r="2" spans="1:16" ht="13">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1249,24 +1413,24 @@
         <v>0</v>
       </c>
       <c r="F2" s="8">
-        <v>6455.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="12.75">
+        <v>6457.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="13">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="4">
         <f>(-F2/F3)</f>
-        <v>3469.2605331040413</v>
+        <v>3441.5369857173309</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="8">
-        <v>-1.8608</v>
+        <v>-1.8764000000000001</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>4</v>
@@ -1275,14 +1439,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="12.75">
+    <row r="4" spans="1:16" ht="13">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5">
         <f>B6+C3</f>
-        <v>42063.260533104039</v>
+        <v>42035.536985717328</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1293,7 +1457,7 @@
         <v>42078.989200863929</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="12.75">
+    <row r="5" spans="1:16" ht="13">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1306,7 +1470,7 @@
         <v>42063.260533104039</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="12.75">
+    <row r="6" spans="1:16" ht="13">
       <c r="A6" s="3"/>
       <c r="B6" s="6">
         <v>38594</v>
@@ -1314,10 +1478,14 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-    </row>
-    <row r="7" spans="1:16" ht="12.75">
+      <c r="O6" s="12">
+        <v>39191</v>
+      </c>
+      <c r="P6" s="13">
+        <v>41938.898908940486</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="13">
       <c r="A7" s="3"/>
       <c r="B7" s="9">
         <v>38594</v>
@@ -1330,10 +1498,14 @@
         <v>6487.82</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-    </row>
-    <row r="8" spans="1:16" ht="12.75">
+      <c r="O7" s="12">
+        <v>39218</v>
+      </c>
+      <c r="P7" s="13">
+        <v>42035.536985717328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="13">
       <c r="A8" s="3"/>
       <c r="B8" s="9">
         <v>38624</v>
@@ -1349,7 +1521,7 @@
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16" ht="12.75">
+    <row r="9" spans="1:16" ht="13">
       <c r="A9" s="3"/>
       <c r="B9" s="9">
         <v>38655</v>
@@ -1365,7 +1537,7 @@
       <c r="O9" s="11"/>
       <c r="P9" s="11"/>
     </row>
-    <row r="10" spans="1:16" ht="12.75">
+    <row r="10" spans="1:16" ht="13">
       <c r="A10" s="3"/>
       <c r="B10" s="9">
         <v>38685</v>
@@ -1381,7 +1553,7 @@
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
     </row>
-    <row r="11" spans="1:16" ht="12.75">
+    <row r="11" spans="1:16" ht="13">
       <c r="A11" s="3"/>
       <c r="B11" s="9">
         <v>38716</v>
@@ -1397,7 +1569,7 @@
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
     </row>
-    <row r="12" spans="1:16" ht="12.75">
+    <row r="12" spans="1:16" ht="13">
       <c r="A12" s="3"/>
       <c r="B12" s="9">
         <v>38747</v>
@@ -1413,7 +1585,7 @@
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="1:16" ht="12.75">
+    <row r="13" spans="1:16" ht="13">
       <c r="A13" s="3"/>
       <c r="B13" s="9">
         <v>38775</v>
@@ -1429,7 +1601,7 @@
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
     </row>
-    <row r="14" spans="1:16" ht="12.75">
+    <row r="14" spans="1:16" ht="13">
       <c r="A14" s="3"/>
       <c r="B14" s="9">
         <v>38806</v>
@@ -1442,8 +1614,10 @@
         <v>6120.7</v>
       </c>
       <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:16" ht="12.75">
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+    </row>
+    <row r="15" spans="1:16" ht="13">
       <c r="A15" s="3"/>
       <c r="B15" s="9">
         <v>38836</v>
@@ -1457,7 +1631,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:16" ht="12.75">
+    <row r="16" spans="1:16" ht="13">
       <c r="A16" s="3"/>
       <c r="B16" s="9">
         <v>38867</v>
@@ -1471,7 +1645,7 @@
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="12.75">
+    <row r="17" spans="1:5" ht="13">
       <c r="A17" s="3"/>
       <c r="B17" s="9">
         <v>38897</v>
@@ -1485,7 +1659,7 @@
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="12.75">
+    <row r="18" spans="1:5" ht="13">
       <c r="A18" s="3"/>
       <c r="B18" s="9">
         <v>38928</v>
@@ -1499,7 +1673,7 @@
       </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="12.75">
+    <row r="19" spans="1:5" ht="13">
       <c r="A19" s="3"/>
       <c r="B19" s="9">
         <v>38959</v>
@@ -1513,7 +1687,7 @@
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="12.75">
+    <row r="20" spans="1:5" ht="13">
       <c r="A20" s="3"/>
       <c r="B20" s="9">
         <v>38989</v>
@@ -1527,7 +1701,7 @@
       </c>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="12.75">
+    <row r="21" spans="1:5" ht="13">
       <c r="A21" s="3"/>
       <c r="B21" s="9">
         <v>39020</v>
@@ -1541,7 +1715,7 @@
       </c>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" ht="12.75">
+    <row r="22" spans="1:5" ht="13">
       <c r="A22" s="3"/>
       <c r="B22" s="9">
         <v>39050</v>
@@ -1555,7 +1729,7 @@
       </c>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="12.75">
+    <row r="23" spans="1:5" ht="13">
       <c r="A23" s="3"/>
       <c r="B23" s="9">
         <v>39081</v>
@@ -1569,7 +1743,7 @@
       </c>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" ht="12.75">
+    <row r="24" spans="1:5" ht="13">
       <c r="A24" s="3"/>
       <c r="B24" s="9">
         <v>39112</v>
@@ -1583,97 +1757,130 @@
       </c>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" ht="12.75">
+    <row r="25" spans="1:5" ht="13">
       <c r="A25" s="3"/>
       <c r="B25" s="9">
-        <v>39133</v>
+        <v>39140</v>
       </c>
       <c r="C25" s="7">
         <f t="shared" ref="C25" si="2">B25-$B$6</f>
-        <v>539</v>
+        <v>546</v>
       </c>
       <c r="D25" s="10">
-        <v>5472.57</v>
+        <v>5399.57</v>
       </c>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" ht="12.75">
+    <row r="26" spans="1:5" ht="13">
       <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
+      <c r="B26" s="9">
+        <v>39171</v>
+      </c>
+      <c r="C26" s="7">
+        <f t="shared" ref="C26:C28" si="3">B26-$B$6</f>
+        <v>577</v>
+      </c>
+      <c r="D26" s="10">
+        <v>5328.18</v>
+      </c>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" ht="12.75">
+    <row r="27" spans="1:5" ht="13">
       <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
+      <c r="B27" s="9">
+        <v>39201</v>
+      </c>
+      <c r="C27" s="7">
+        <f t="shared" ref="C27" si="4">B27-$B$6</f>
+        <v>607</v>
+      </c>
+      <c r="D27" s="10">
+        <v>5395.66</v>
+      </c>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" ht="12.75">
+    <row r="28" spans="1:5" ht="13">
       <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
+      <c r="B28" s="9">
+        <v>39218</v>
+      </c>
+      <c r="C28" s="7">
+        <f t="shared" si="3"/>
+        <v>624</v>
+      </c>
+      <c r="D28" s="10">
+        <v>5277.08</v>
+      </c>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" ht="12.75">
+    <row r="29" spans="1:5" ht="13">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" ht="12.75">
+    <row r="30" spans="1:5" ht="13">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" ht="12.75">
+    <row r="31" spans="1:5" ht="13">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" ht="12.75">
+    <row r="32" spans="1:5" ht="13">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" ht="12.75">
+    <row r="33" spans="1:5" ht="13">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" ht="12.75">
+    <row r="34" spans="1:5" ht="13">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="35" spans="1:5" ht="13">
+      <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" ht="20" customHeight="1">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
     </row>
+    <row r="37" spans="1:5" ht="20" customHeight="1">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.25" footer="0.25"/>
-  <pageSetup orientation="landscape" useFirstPageNumber="1" r:id="rId1"/>
+  <pageSetup orientation="landscape" useFirstPageNumber="1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Before changing my interests
</commit_message>
<xml_diff>
--- a/vending/Vending Pay-Off.xlsx
+++ b/vending/Vending Pay-Off.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21105"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="-29960" windowWidth="40380" windowHeight="28880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Table 1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <numFmt numFmtId="164" formatCode="mmm\ d\,\ yyyy\ h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="mmm\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -76,8 +76,13 @@
       <color theme="11"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,8 +107,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF1DE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -141,8 +158,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCDCDCD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFCDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCDCDCD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
@@ -194,8 +239,68 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -236,8 +341,17 @@
     <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -246,6 +360,16 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -254,6 +378,16 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -430,10 +564,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$C$7:$C$30</c:f>
+              <c:f>'Sheet 1 - Table 1'!$C$7:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -498,17 +632,23 @@
                   <c:v>607.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>624.0</c:v>
+                  <c:v>638.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>668.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>690.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$D$7:$D$30</c:f>
+              <c:f>'Sheet 1 - Table 1'!$D$7:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>6487.82</c:v>
                 </c:pt>
@@ -574,6 +714,12 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>5277.08</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5089.11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5142.46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -588,11 +734,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="769343592"/>
-        <c:axId val="769346952"/>
+        <c:axId val="640023592"/>
+        <c:axId val="640027032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="769343592"/>
+        <c:axId val="640023592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -627,12 +773,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="769346952"/>
+        <c:crossAx val="640027032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="769346952"/>
+        <c:axId val="640027032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -675,7 +821,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="769343592"/>
+        <c:crossAx val="640023592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1300.0"/>
@@ -775,12 +921,17 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$O$4:$O$9</c:f>
+              <c:f>'Sheet 1 - Table 1'!$O$4:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>39098.0</c:v>
                 </c:pt>
@@ -792,16 +943,22 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>39218.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39261.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39284.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$P$4:$P$9</c:f>
+              <c:f>'Sheet 1 - Table 1'!$P$4:$P$11</c:f>
               <c:numCache>
                 <c:formatCode>mmm\ d\,\ yyyy\ h:mm:ss\ AM/PM</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>42078.98920086393</c:v>
                 </c:pt>
@@ -813,6 +970,12 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>42035.53698571733</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41980.13031636287</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41977.50429139627</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -827,11 +990,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="795896056"/>
-        <c:axId val="795902136"/>
+        <c:axId val="640064392"/>
+        <c:axId val="640070072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="795896056"/>
+        <c:axId val="640064392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -886,12 +1049,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="795902136"/>
+        <c:crossAx val="640070072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="795902136"/>
+        <c:axId val="640070072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -946,7 +1109,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="795896056"/>
+        <c:crossAx val="640064392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1378,10 +1541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1413,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="8">
-        <v>6457.7</v>
+        <v>6465.2</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="13">
@@ -1423,14 +1586,14 @@
       </c>
       <c r="C3" s="4">
         <f>(-F2/F3)</f>
-        <v>3441.5369857173309</v>
+        <v>3383.5042913962734</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="8">
-        <v>-1.8764000000000001</v>
+        <v>-1.9108000000000001</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>4</v>
@@ -1446,7 +1609,7 @@
       </c>
       <c r="C4" s="5">
         <f>B6+C3</f>
-        <v>42035.536985717328</v>
+        <v>41977.504291396275</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1518,8 +1681,12 @@
         <v>6424.82</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
+      <c r="O8" s="12">
+        <v>39261</v>
+      </c>
+      <c r="P8" s="13">
+        <v>41980.130316362876</v>
+      </c>
     </row>
     <row r="9" spans="1:16" ht="13">
       <c r="A9" s="3"/>
@@ -1534,8 +1701,12 @@
         <v>6318.18</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
+      <c r="O9" s="12">
+        <v>39284</v>
+      </c>
+      <c r="P9" s="13">
+        <v>41977.504291396275</v>
+      </c>
     </row>
     <row r="10" spans="1:16" ht="13">
       <c r="A10" s="3"/>
@@ -1630,6 +1801,8 @@
         <v>6026.78</v>
       </c>
       <c r="E15" s="4"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
     </row>
     <row r="16" spans="1:16" ht="13">
       <c r="A16" s="3"/>
@@ -1644,6 +1817,8 @@
         <v>5938.66</v>
       </c>
       <c r="E16" s="4"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
     </row>
     <row r="17" spans="1:5" ht="13">
       <c r="A17" s="3"/>
@@ -1777,7 +1952,7 @@
         <v>39171</v>
       </c>
       <c r="C26" s="7">
-        <f t="shared" ref="C26:C28" si="3">B26-$B$6</f>
+        <f t="shared" ref="C26:C30" si="3">B26-$B$6</f>
         <v>577</v>
       </c>
       <c r="D26" s="10">
@@ -1791,7 +1966,7 @@
         <v>39201</v>
       </c>
       <c r="C27" s="7">
-        <f t="shared" ref="C27" si="4">B27-$B$6</f>
+        <f t="shared" ref="C27:C28" si="4">B27-$B$6</f>
         <v>607</v>
       </c>
       <c r="D27" s="10">
@@ -1802,11 +1977,11 @@
     <row r="28" spans="1:5" ht="13">
       <c r="A28" s="3"/>
       <c r="B28" s="9">
-        <v>39218</v>
+        <v>39232</v>
       </c>
       <c r="C28" s="7">
-        <f t="shared" si="3"/>
-        <v>624</v>
+        <f t="shared" si="4"/>
+        <v>638</v>
       </c>
       <c r="D28" s="10">
         <v>5277.08</v>
@@ -1815,16 +1990,29 @@
     </row>
     <row r="29" spans="1:5" ht="13">
       <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
+      <c r="B29" s="14">
+        <v>39262</v>
+      </c>
+      <c r="C29" s="15">
+        <v>668</v>
+      </c>
+      <c r="D29" s="16">
+        <v>5089.1099999999997</v>
+      </c>
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" ht="13">
       <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
+      <c r="B30" s="9">
+        <v>39284</v>
+      </c>
+      <c r="C30" s="7">
+        <f t="shared" si="3"/>
+        <v>690</v>
+      </c>
+      <c r="D30" s="10">
+        <v>5142.46</v>
+      </c>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" ht="13">
@@ -1871,6 +2059,16 @@
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" ht="20" customHeight="1">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" ht="20" customHeight="1">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
After making color swatches
</commit_message>
<xml_diff>
--- a/vending/Vending Pay-Off.xlsx
+++ b/vending/Vending Pay-Off.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23206"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23480"/>
+    <workbookView xWindow="160" yWindow="-26540" windowWidth="38400" windowHeight="23480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Table 1" sheetId="1" r:id="rId1"/>
@@ -202,8 +202,140 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="113">
+  <cellStyleXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -600,7 +732,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="113">
+  <cellStyles count="157">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -657,6 +789,28 @@
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -713,6 +867,28 @@
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -889,10 +1065,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$C$7:$C$45</c:f>
+              <c:f>'Sheet 1 - Table 1'!$C$7:$C$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -1000,16 +1176,34 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>1109.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1181.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1218.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1249.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1277.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1290.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1354.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$D$7:$D$45</c:f>
+              <c:f>'Sheet 1 - Table 1'!$D$7:$D$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>6487.82</c:v>
                 </c:pt>
@@ -1117,6 +1311,24 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>4506.83</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4472.03</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4398.9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4373.86</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4252.75</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4161.33</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4034.23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1131,11 +1343,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2053901672"/>
-        <c:axId val="2053903096"/>
+        <c:axId val="2141227960"/>
+        <c:axId val="2141223096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2053901672"/>
+        <c:axId val="2141227960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1170,12 +1382,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2053903096"/>
+        <c:crossAx val="2141223096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2053903096"/>
+        <c:axId val="2141223096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1218,7 +1430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2053901672"/>
+        <c:crossAx val="2141227960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1300.0"/>
@@ -1325,10 +1537,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$O$4:$O$18</c:f>
+              <c:f>'Sheet 1 - Table 1'!$O$4:$O$22</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>39098.0</c:v>
                 </c:pt>
@@ -1367,16 +1579,31 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>39703.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39775.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39829.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39870.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>39884.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39948.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$P$4:$P$18</c:f>
+              <c:f>'Sheet 1 - Table 1'!$P$4:$P$22</c:f>
               <c:numCache>
                 <c:formatCode>mmm\ d\,\ yyyy\ h:mm:ss\ AM/PM</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>42078.98920086393</c:v>
                 </c:pt>
@@ -1415,6 +1642,21 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>42608.38261524934</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42594.6882743086</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42565.57398148148</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42545.55218169474</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42510.88565666442</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42473.26969348891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1429,11 +1671,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2135612344"/>
-        <c:axId val="2135618024"/>
+        <c:axId val="-2146958520"/>
+        <c:axId val="-2146952840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2135612344"/>
+        <c:axId val="-2146958520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1488,12 +1730,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2135618024"/>
+        <c:crossAx val="-2146952840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2135618024"/>
+        <c:axId val="-2146952840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1548,7 +1790,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2135612344"/>
+        <c:crossAx val="-2146958520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1609,7 +1851,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>226218</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>214313</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1980,10 +2222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2015,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="8">
-        <v>6391.7</v>
+        <v>6416.7</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="13">
@@ -2025,14 +2267,14 @@
       </c>
       <c r="C3" s="4">
         <f>(-F2/F3)</f>
-        <v>4014.3826152493402</v>
+        <v>3879.2696934889063</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="8">
-        <v>-1.5922000000000001</v>
+        <v>-1.6540999999999999</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>4</v>
@@ -2048,7 +2290,7 @@
       </c>
       <c r="C4" s="5">
         <f>B6+C3</f>
-        <v>42608.382615249342</v>
+        <v>42473.26969348891</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -2300,8 +2542,12 @@
         <v>5880.67</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
+      <c r="O17" s="12">
+        <v>39775</v>
+      </c>
+      <c r="P17" s="13">
+        <v>42594.688274308595</v>
+      </c>
     </row>
     <row r="18" spans="1:16" ht="13">
       <c r="A18" s="3"/>
@@ -2316,8 +2562,12 @@
         <v>5804.99</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
+      <c r="O18" s="12">
+        <v>39829</v>
+      </c>
+      <c r="P18" s="13">
+        <v>42565.573981481481</v>
+      </c>
     </row>
     <row r="19" spans="1:16" ht="13">
       <c r="A19" s="3"/>
@@ -2332,8 +2582,12 @@
         <v>5762.59</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
+      <c r="O19" s="12">
+        <v>39870</v>
+      </c>
+      <c r="P19" s="13">
+        <v>42545.552181694744</v>
+      </c>
     </row>
     <row r="20" spans="1:16" ht="13">
       <c r="A20" s="3"/>
@@ -2348,8 +2602,12 @@
         <v>5727.76</v>
       </c>
       <c r="E20" s="4"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
+      <c r="O20" s="12">
+        <v>39884</v>
+      </c>
+      <c r="P20" s="13">
+        <v>42510.885656664424</v>
+      </c>
     </row>
     <row r="21" spans="1:16" ht="13">
       <c r="A21" s="3"/>
@@ -2364,8 +2622,12 @@
         <v>5677.22</v>
       </c>
       <c r="E21" s="4"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
+      <c r="O21" s="12">
+        <v>39948</v>
+      </c>
+      <c r="P21" s="13">
+        <v>42473.26969348891</v>
+      </c>
     </row>
     <row r="22" spans="1:16" ht="13">
       <c r="A22" s="3"/>
@@ -2412,6 +2674,8 @@
         <v>5458.44</v>
       </c>
       <c r="E24" s="4"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
     </row>
     <row r="25" spans="1:16" ht="13">
       <c r="A25" s="3"/>
@@ -2426,6 +2690,8 @@
         <v>5399.57</v>
       </c>
       <c r="E25" s="4"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
     </row>
     <row r="26" spans="1:16" ht="13">
       <c r="A26" s="3"/>
@@ -2440,6 +2706,8 @@
         <v>5328.18</v>
       </c>
       <c r="E26" s="4"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
     </row>
     <row r="27" spans="1:16" ht="13">
       <c r="A27" s="3"/>
@@ -2454,6 +2722,8 @@
         <v>5395.66</v>
       </c>
       <c r="E27" s="4"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
     </row>
     <row r="28" spans="1:16" ht="13">
       <c r="A28" s="3"/>
@@ -2576,7 +2846,7 @@
         <v>39477</v>
       </c>
       <c r="C36" s="7">
-        <f t="shared" ref="C36:C42" si="8">B36-$B$6</f>
+        <f t="shared" ref="C36:C48" si="8">B36-$B$6</f>
         <v>883</v>
       </c>
       <c r="D36" s="10">
@@ -2660,7 +2930,7 @@
         <v>39703</v>
       </c>
       <c r="C42" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="C42:C47" si="9">B42-$B$6</f>
         <v>1109</v>
       </c>
       <c r="D42" s="16">
@@ -2668,35 +2938,89 @@
       </c>
       <c r="E42" s="15"/>
     </row>
-    <row r="44" spans="1:5" ht="20" customHeight="1">
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:5" ht="20" customHeight="1">
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="1:5" ht="20" customHeight="1">
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:5" ht="20" customHeight="1">
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:5" ht="20" customHeight="1">
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="2:4" ht="20" customHeight="1">
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
+    <row r="43" spans="1:5" ht="13">
+      <c r="A43" s="17"/>
+      <c r="B43" s="18">
+        <v>39775</v>
+      </c>
+      <c r="C43" s="7">
+        <f t="shared" si="9"/>
+        <v>1181</v>
+      </c>
+      <c r="D43" s="16">
+        <v>4472.03</v>
+      </c>
+      <c r="E43" s="15"/>
+    </row>
+    <row r="44" spans="1:5" ht="13">
+      <c r="A44" s="17"/>
+      <c r="B44" s="18">
+        <v>39812</v>
+      </c>
+      <c r="C44" s="7">
+        <f t="shared" si="9"/>
+        <v>1218</v>
+      </c>
+      <c r="D44" s="16">
+        <v>4398.8999999999996</v>
+      </c>
+      <c r="E44" s="15"/>
+    </row>
+    <row r="45" spans="1:5" ht="13">
+      <c r="A45" s="17"/>
+      <c r="B45" s="18">
+        <v>39843</v>
+      </c>
+      <c r="C45" s="7">
+        <f t="shared" ref="C45" si="10">B45-$B$6</f>
+        <v>1249</v>
+      </c>
+      <c r="D45" s="16">
+        <v>4373.8599999999997</v>
+      </c>
+      <c r="E45" s="15"/>
+    </row>
+    <row r="46" spans="1:5" ht="13">
+      <c r="A46" s="17"/>
+      <c r="B46" s="18">
+        <v>39871</v>
+      </c>
+      <c r="C46" s="7">
+        <f t="shared" si="9"/>
+        <v>1277</v>
+      </c>
+      <c r="D46" s="16">
+        <v>4252.75</v>
+      </c>
+      <c r="E46" s="15"/>
+    </row>
+    <row r="47" spans="1:5" ht="13">
+      <c r="A47" s="17"/>
+      <c r="B47" s="18">
+        <v>39884</v>
+      </c>
+      <c r="C47" s="7">
+        <f t="shared" si="9"/>
+        <v>1290</v>
+      </c>
+      <c r="D47" s="16">
+        <v>4161.33</v>
+      </c>
+      <c r="E47" s="15"/>
+    </row>
+    <row r="48" spans="1:5" ht="13">
+      <c r="A48" s="17"/>
+      <c r="B48" s="18">
+        <v>39948</v>
+      </c>
+      <c r="C48" s="7">
+        <f t="shared" si="8"/>
+        <v>1354</v>
+      </c>
+      <c r="D48" s="16">
+        <v>4034.23</v>
+      </c>
+      <c r="E48" s="15"/>
     </row>
     <row r="50" spans="2:4" ht="20" customHeight="1">
       <c r="B50" s="4"/>
@@ -2712,6 +3036,36 @@
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="2:4" ht="20" customHeight="1">
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="2:4" ht="20" customHeight="1">
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+    </row>
+    <row r="55" spans="2:4" ht="20" customHeight="1">
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+    </row>
+    <row r="56" spans="2:4" ht="20" customHeight="1">
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+    </row>
+    <row r="57" spans="2:4" ht="20" customHeight="1">
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="2:4" ht="20" customHeight="1">
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
getting ready to switch to git
</commit_message>
<xml_diff>
--- a/vending/Vending Pay-Off.xlsx
+++ b/vending/Vending Pay-Off.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23812"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="-30500" windowWidth="38400" windowHeight="23480"/>
@@ -202,8 +202,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="177">
+  <cellStyleXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -792,7 +822,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="177">
+  <cellStyles count="187">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -881,6 +911,11 @@
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -969,6 +1004,11 @@
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1145,10 +1185,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$C$7:$C$53</c:f>
+              <c:f>'Sheet 1 - Table 1'!$C$7:$C$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="47"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -1279,17 +1319,20 @@
                   <c:v>1461.0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1486.0</c:v>
+                  <c:v>1491.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1509.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$D$7:$D$53</c:f>
+              <c:f>'Sheet 1 - Table 1'!$D$7:$D$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="47"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>6487.82</c:v>
                 </c:pt>
@@ -1420,7 +1463,10 @@
                   <c:v>4095.72</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3923.86</c:v>
+                  <c:v>3917.86</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4245.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1435,11 +1481,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2141282680"/>
-        <c:axId val="2141286008"/>
+        <c:axId val="2061785256"/>
+        <c:axId val="2061781784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2141282680"/>
+        <c:axId val="2061785256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1474,12 +1520,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141286008"/>
+        <c:crossAx val="2061781784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2141286008"/>
+        <c:axId val="2061781784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1522,7 +1568,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141282680"/>
+        <c:crossAx val="2061785256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1300.0"/>
@@ -1629,10 +1675,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$O$4:$O$23</c:f>
+              <c:f>'Sheet 1 - Table 1'!$O$4:$O$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>39098.0</c:v>
                 </c:pt>
@@ -1689,16 +1735,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>40080.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40103.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sheet 1 - Table 1'!$P$4:$P$23</c:f>
+              <c:f>'Sheet 1 - Table 1'!$P$4:$P$24</c:f>
               <c:numCache>
                 <c:formatCode>mmm\ d\,\ yyyy\ h:mm:ss\ AM/PM</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>42078.98920086393</c:v>
                 </c:pt>
@@ -1755,6 +1804,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>42485.99029126213</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42551.51653935185</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1769,11 +1821,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2051736456"/>
-        <c:axId val="2144735992"/>
+        <c:axId val="2135968760"/>
+        <c:axId val="2135963080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2051736456"/>
+        <c:axId val="2135968760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1828,12 +1880,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144735992"/>
+        <c:crossAx val="2135963080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2144735992"/>
+        <c:axId val="2135963080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1888,7 +1940,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2051736456"/>
+        <c:crossAx val="2135968760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2320,10 +2372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2355,7 +2407,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="8">
-        <v>6414</v>
+        <v>6399.7</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="13">
@@ -2365,14 +2417,14 @@
       </c>
       <c r="C3" s="4">
         <f>(-F2/F3)</f>
-        <v>3891.990291262136</v>
+        <v>3957.5165419578257</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="8">
-        <v>-1.6479999999999999</v>
+        <v>-1.6171</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>4</v>
@@ -2388,7 +2440,7 @@
       </c>
       <c r="C4" s="5">
         <f>B6+C3</f>
-        <v>42485.990291262133</v>
+        <v>42551.516541957826</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -2760,8 +2812,12 @@
         <v>5536.02</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
+      <c r="O23" s="12">
+        <v>40103</v>
+      </c>
+      <c r="P23" s="13">
+        <v>42551.516539351855</v>
+      </c>
     </row>
     <row r="24" spans="1:16" ht="13">
       <c r="A24" s="3"/>
@@ -2855,6 +2911,8 @@
         <v>5089.1099999999997</v>
       </c>
       <c r="E29" s="4"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
     </row>
     <row r="30" spans="1:16" ht="13">
       <c r="A30" s="3"/>
@@ -2950,7 +3008,7 @@
         <v>39477</v>
       </c>
       <c r="C36" s="7">
-        <f t="shared" ref="C36:C50" si="8">B36-$B$6</f>
+        <f t="shared" ref="C36:C51" si="8">B36-$B$6</f>
         <v>883</v>
       </c>
       <c r="D36" s="10">
@@ -3034,7 +3092,7 @@
         <v>39703</v>
       </c>
       <c r="C42" s="7">
-        <f t="shared" ref="C42:C49" si="9">B42-$B$6</f>
+        <f t="shared" ref="C42:C48" si="9">B42-$B$6</f>
         <v>1109</v>
       </c>
       <c r="D42" s="16">
@@ -3132,7 +3190,7 @@
         <v>40055</v>
       </c>
       <c r="C49" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="C49:C50" si="11">B49-$B$6</f>
         <v>1461</v>
       </c>
       <c r="D49" s="16">
@@ -3143,21 +3201,30 @@
     <row r="50" spans="1:5" ht="13">
       <c r="A50" s="17"/>
       <c r="B50" s="18">
-        <v>40080</v>
+        <v>40085</v>
       </c>
       <c r="C50" s="7">
+        <f t="shared" si="11"/>
+        <v>1491</v>
+      </c>
+      <c r="D50" s="16">
+        <v>3917.86</v>
+      </c>
+      <c r="E50" s="15"/>
+    </row>
+    <row r="51" spans="1:5" ht="13">
+      <c r="A51" s="17"/>
+      <c r="B51" s="18">
+        <v>40103</v>
+      </c>
+      <c r="C51" s="7">
         <f t="shared" si="8"/>
-        <v>1486</v>
-      </c>
-      <c r="D50" s="16">
-        <v>3923.86</v>
-      </c>
-      <c r="E50" s="15"/>
-    </row>
-    <row r="52" spans="1:5" ht="20" customHeight="1">
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
+        <v>1509</v>
+      </c>
+      <c r="D51" s="16">
+        <v>4245.16</v>
+      </c>
+      <c r="E51" s="15"/>
     </row>
     <row r="53" spans="1:5" ht="20" customHeight="1">
       <c r="B53" s="4"/>
@@ -3198,6 +3265,11 @@
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
+    </row>
+    <row r="61" spans="1:5" ht="20" customHeight="1">
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.25" footer="0.25"/>

</xml_diff>